<commit_message>
Version 0.8: Se finaliza el desarrollo, se unenen todas las paginas, se realiza logica para el login, cambio de contraseña y recuperacion de contraseñas se ajusta base de datos
</commit_message>
<xml_diff>
--- a/views/assets/plantilla/estudiante_rubrica_pruebas.xlsx
+++ b/views/assets/plantilla/estudiante_rubrica_pruebas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhurrea\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rubrica\views\assets\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,8 +18,142 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Javier Hernando Urrea Bejarano</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CC: Cédula de Ciudadanía
+TI: Tarjeta de Identidad
+CE: Cédula de Extranjería
+PAS: Pasaporte
+OTRO: Otro</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo para posgrados</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo para posgrados</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SI
+NO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ID del programa que se encuentra en el listado d eprogramas del aplicativo
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo para programa de medicina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Solo para programa de medicina
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo para programas de posgrados</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solo para programas de posgrados</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>cedula</t>
   </si>
@@ -48,18 +182,9 @@
     <t>Bogotá</t>
   </si>
   <si>
-    <t>A nada</t>
-  </si>
-  <si>
-    <t>A nad</t>
-  </si>
-  <si>
     <t>javier pruebas Fucs 2</t>
   </si>
   <si>
-    <t>Ninguno</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
@@ -108,17 +233,17 @@
     <t>FUCS</t>
   </si>
   <si>
-    <t>Abogada</t>
-  </si>
-  <si>
-    <t>ing. Nuclear</t>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +378,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -435,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -550,6 +687,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -595,8 +747,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -917,60 +1070,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -999,10 +1169,10 @@
         <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -1010,7 +1180,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1022,66 +1192,33 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>2022</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1023</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>2020</v>
-      </c>
-      <c r="H4">
-        <v>412</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4">
-        <v>36</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>